<commit_message>
Remove old named ranges from example
</commit_message>
<xml_diff>
--- a/src/test/resources/test-suites/export/daysbug/expected.xlsx
+++ b/src/test/resources/test-suites/export/daysbug/expected.xlsx
@@ -1,61 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirsten/Development/molnify-xlport/src/test/resources/test-suites/export/daysbug/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\peter\repos\xlport\src\test\resources\test-suites\export\daysbug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E018B1F-5468-E741-A3EC-66FCB3CE151B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731150FA-3968-47C0-863D-C6B46191B417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="460" windowWidth="18000" windowHeight="27260" xr2:uid="{D2687B94-08F0-4321-B5D3-80C7CCDCB67F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="16776" xr2:uid="{D2687B94-08F0-4321-B5D3-80C7CCDCB67F}"/>
   </bookViews>
   <sheets>
     <sheet name="Deal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="Account">Deal!#REF!</definedName>
-    <definedName name="Account_Number">Deal!#REF!</definedName>
-    <definedName name="ActionPitchRound1">Deal!#REF!</definedName>
-    <definedName name="ActionPitchRound2">Deal!#REF!</definedName>
-    <definedName name="ActionPitchRound3">Deal!#REF!</definedName>
-    <definedName name="ActionTender">Deal!#REF!</definedName>
-    <definedName name="Category">Deal!#REF!</definedName>
-    <definedName name="ClientProjectCode">Deal!#REF!</definedName>
-    <definedName name="Contact">Deal!#REF!</definedName>
-    <definedName name="Country">Deal!#REF!</definedName>
-    <definedName name="DealName">Deal!#REF!</definedName>
-    <definedName name="DiscountedBudget">Deal!#REF!</definedName>
-    <definedName name="ExistencePitchRound1">Deal!#REF!</definedName>
-    <definedName name="ExistencePitchRound2">Deal!#REF!</definedName>
-    <definedName name="ExistencePitchRound3">Deal!#REF!</definedName>
-    <definedName name="ExistenceTender">Deal!#REF!</definedName>
-    <definedName name="Function">Deal!#REF!</definedName>
-    <definedName name="Industry">Deal!#REF!</definedName>
-    <definedName name="KeyAccount">Deal!#REF!</definedName>
-    <definedName name="Leads">Deal!#REF!</definedName>
-    <definedName name="NameCompetitor1">Deal!#REF!</definedName>
-    <definedName name="NameCompetitor2">Deal!#REF!</definedName>
-    <definedName name="NameCompetitor3">Deal!#REF!</definedName>
-    <definedName name="NextSteps">Deal!#REF!</definedName>
-    <definedName name="Probability">Deal!#REF!</definedName>
-    <definedName name="ProjectEnd">Deal!#REF!</definedName>
-    <definedName name="ProjectNumber">Deal!#REF!</definedName>
-    <definedName name="ProjectStart">Deal!#REF!</definedName>
-    <definedName name="ResultPitchRound1">Deal!#REF!</definedName>
-    <definedName name="ResultPitchRound2">Deal!#REF!</definedName>
-    <definedName name="ResultPitchRound3">Deal!#REF!</definedName>
-    <definedName name="ResultTender">Deal!#REF!</definedName>
-    <definedName name="Status">Deal!#REF!</definedName>
-    <definedName name="StatusCompetitor1">Deal!#REF!</definedName>
-    <definedName name="StatusCompetitor2">Deal!#REF!</definedName>
-    <definedName name="StatusCompetitor3">Deal!#REF!</definedName>
-    <definedName name="StratImportance">Deal!#REF!</definedName>
-    <definedName name="TemplateType">Deal!#REF!</definedName>
-    <definedName name="UndiscountedBudget">Deal!#REF!</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -242,9 +206,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,7 +246,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -388,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,7 +494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,29 +505,31 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>21</v>
       </c>
@@ -571,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>1</v>
       </c>

</xml_diff>